<commit_message>
Seperated PIT vs Match data collection also updated template and worksheet creating to include pit scout data
</commit_message>
<xml_diff>
--- a/ScoutLeaderScripts/ScoutingData_template.xlsx
+++ b/ScoutLeaderScripts/ScoutingData_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>Team Number</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>What can they do in end game</t>
-  </si>
-  <si>
-    <t>What can they do in autonmous</t>
-  </si>
-  <si>
     <t>Pit Scouting</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Bumper Height</t>
   </si>
   <si>
-    <t>Where can they place cubes</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -250,6 +241,12 @@
   </si>
   <si>
     <t>Min Results</t>
+  </si>
+  <si>
+    <t>Pit Scouter Notes</t>
+  </si>
+  <si>
+    <t>Pit Scout Results</t>
   </si>
 </sst>
 </file>
@@ -322,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -397,15 +394,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -444,14 +432,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -756,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,69 +780,76 @@
     <col min="26" max="26" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="4" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="4" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:28" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18" t="s">
+    <row r="6" spans="1:30" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AD6" s="20"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
@@ -896,8 +891,10 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="16"/>
       <c r="AB7" s="17"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="17"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -914,13 +911,13 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>8</v>
@@ -950,13 +947,13 @@
         <v>8</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>8</v>
@@ -971,19 +968,25 @@
         <v>8</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AB8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1001,7 +1004,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -1020,8 +1023,9 @@
       <c r="P11" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A8:AB8"/>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC7:AD7"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="F7:I7"/>
@@ -1057,13 +1061,13 @@
         <v>573</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1">
         <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1071,7 +1075,7 @@
         <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1079,7 +1083,7 @@
         <v>94</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1087,7 +1091,7 @@
         <v>835</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1095,7 +1099,7 @@
         <v>1481</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1103,7 +1107,7 @@
         <v>1502</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1111,7 +1115,7 @@
         <v>1701</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1119,7 +1123,7 @@
         <v>2048</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1127,7 +1131,7 @@
         <v>3302</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1135,7 +1139,7 @@
         <v>3538</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1143,7 +1147,7 @@
         <v>3547</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1151,7 +1155,7 @@
         <v>4680</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1159,7 +1163,7 @@
         <v>4737</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1167,7 +1171,7 @@
         <v>4758</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1175,7 +1179,7 @@
         <v>4768</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1183,7 +1187,7 @@
         <v>4838</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.35">
@@ -1191,7 +1195,7 @@
         <v>4840</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.35">
@@ -1199,7 +1203,7 @@
         <v>4854</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.35">
@@ -1207,7 +1211,7 @@
         <v>5065</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.35">
@@ -1215,7 +1219,7 @@
         <v>5167</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.35">
@@ -1223,7 +1227,7 @@
         <v>5197</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.35">
@@ -1231,7 +1235,7 @@
         <v>5217</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.35">
@@ -1239,7 +1243,7 @@
         <v>5436</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.35">
@@ -1247,7 +1251,7 @@
         <v>5467</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.35">
@@ -1255,7 +1259,7 @@
         <v>5531</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.35">
@@ -1263,7 +1267,7 @@
         <v>5619</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.35">
@@ -1271,7 +1275,7 @@
         <v>5642</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.35">
@@ -1279,7 +1283,7 @@
         <v>5843</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.35">
@@ -1287,7 +1291,7 @@
         <v>5901</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.35">
@@ -1295,7 +1299,7 @@
         <v>6057</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="5:6" x14ac:dyDescent="0.35">
@@ -1303,7 +1307,7 @@
         <v>6136</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.35">
@@ -1311,7 +1315,7 @@
         <v>6150</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.35">
@@ -1319,7 +1323,7 @@
         <v>6567</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.35">
@@ -1327,7 +1331,7 @@
         <v>6633</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.35">
@@ -1335,7 +1339,7 @@
         <v>6742</v>
       </c>
       <c r="F35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.35">
@@ -1343,7 +1347,7 @@
         <v>6862</v>
       </c>
       <c r="F36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.35">
@@ -1351,7 +1355,7 @@
         <v>7196</v>
       </c>
       <c r="F37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.35">
@@ -1359,7 +1363,7 @@
         <v>7218</v>
       </c>
       <c r="F38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.35">
@@ -1367,7 +1371,7 @@
         <v>7232</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1394,7 +1398,7 @@
         <v>573</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1407,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,39 +1448,29 @@
       <c r="B2" s="10"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="20"/>
+      <c r="A4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -1530,13 +1524,13 @@
         <v>10</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>8</v>
@@ -1562,7 +1556,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1623,7 +1617,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1666,7 +1660,7 @@
     </row>
     <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>

</xml_diff>

<commit_message>
Included image addition and resize code
</commit_message>
<xml_diff>
--- a/ScoutLeaderScripts/ScoutingData_template.xlsx
+++ b/ScoutLeaderScripts/ScoutingData_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11870" windowHeight="6100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11870" windowHeight="6100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,11 +435,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -746,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
@@ -811,87 +811,87 @@
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:30" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="W6" s="20"/>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="20" t="s">
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="AD6" s="20"/>
+      <c r="AD6" s="15"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="15" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="15" t="s">
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
       <c r="U7" s="17"/>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="15" t="s">
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
       <c r="AB7" s="17"/>
-      <c r="AC7" s="15"/>
+      <c r="AC7" s="16"/>
       <c r="AD7" s="17"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
@@ -1411,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,10 +1448,10 @@
       <c r="B2" s="10"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="20"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1468,6 +1468,7 @@
         <v>72</v>
       </c>
     </row>
+    <row r="9" spans="1:18" ht="112" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>25</v>
@@ -1477,25 +1478,25 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
       <c r="Q12" s="17"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>